<commit_message>
Exclude AGRCO2P from CB and emission constraint
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8445B910-2F87-4895-8F92-B5DAF5B51ABC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA56CBD3-6542-4AE6-BC9B-611DAB1C7358}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -336,10 +336,10 @@
     <t>NET</t>
   </si>
   <si>
-    <t>*CO2*,-*CO2S</t>
-  </si>
-  <si>
     <t>ENV</t>
+  </si>
+  <si>
+    <t>*CO2*,-*CO2S,-AGRCO2P</t>
   </si>
 </sst>
 </file>
@@ -1847,15 +1847,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="9.140625" style="8"/>
     <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
@@ -1988,7 +1988,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1996,7 +1996,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C5, config!$B$4:$C$12,2,FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
+        <v>*CO2*,-*CO2S,-AGRCO2P</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>VLOOKUP(D5, config!$B$4:$C$12,2,FALSE)</f>
@@ -2238,7 +2238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C5, config!$B$4:$C$12,2,FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
+        <v>*CO2*,-*CO2S,-AGRCO2P</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>VLOOKUP(D5, config!$B$4:$C$12,2,FALSE)</f>

</xml_diff>

<commit_message>
Remove AGRCO2P as CO2eq emission in AGR
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA56CBD3-6542-4AE6-BC9B-611DAB1C7358}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77E2926-3E88-4E66-8AA5-797972EE4164}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -339,7 +339,7 @@
     <t>ENV</t>
   </si>
   <si>
-    <t>*CO2*,-*CO2S,-AGRCO2P</t>
+    <t>*CO2*,-*CO2S</t>
   </si>
 </sst>
 </file>
@@ -1847,7 +1847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C5, config!$B$4:$C$12,2,FALSE)</f>
-        <v>*CO2*,-*CO2S,-AGRCO2P</v>
+        <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>VLOOKUP(D5, config!$B$4:$C$12,2,FALSE)</f>
@@ -2238,7 +2238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C5, config!$B$4:$C$12,2,FALSE)</f>
-        <v>*CO2*,-*CO2S,-AGRCO2P</v>
+        <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>VLOOKUP(D5, config!$B$4:$C$12,2,FALSE)</f>

</xml_diff>

<commit_message>
Exclude international aviation from CB constraint and net-zero constraint
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77E2926-3E88-4E66-8AA5-797972EE4164}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9CF55B-7986-4970-B0AE-A09CEF1D4C6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>LimType</t>
   </si>
@@ -340,6 +340,15 @@
   </si>
   <si>
     <t>*CO2*,-*CO2S</t>
+  </si>
+  <si>
+    <t>UC_CUMFLO</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>T-A*INT*</t>
   </si>
 </sst>
 </file>
@@ -1845,9 +1854,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1985,82 +1994,60 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-    </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
+      <c r="B13" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-1</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
@@ -2095,6 +2082,44 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2103,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,39 +2139,40 @@
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8"/>
-    <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="5" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G4" s="8" t="str">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2157,25 +2183,31 @@
         <v>74</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>72</v>
       </c>
@@ -2185,47 +2217,71 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B5, config!$B$4:$C$12,2,FALSE) &amp; "_Single"</f>
+        <f>VLOOKUP(B5, config!$B$4:$C$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_CB-420Mt_Single</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C5, config!$B$4:$C$12,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D5, config!$B$4:$C$12,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
-      <c r="E7" s="8" t="str">
-        <f>VLOOKUP(E5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="F7" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>2018-2050</v>
       </c>
-      <c r="F7" s="8" t="str">
-        <f>VLOOKUP(F5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="G7" s="8" t="str">
+        <f>VLOOKUP(G5, config!$B$4:$C$14,2,FALSE)</f>
         <v>NET</v>
       </c>
-      <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="H7" s="8" t="str">
+        <f>VLOOKUP(H5, config!$B$4:$C$14,2,FALSE)</f>
         <v>UP</v>
       </c>
-      <c r="H7" s="8">
-        <f>VLOOKUP(H5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="I7" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="I7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$C$12,2,FALSE)*1000</f>
+      <c r="K7" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$C$14,2,FALSE)*1000</f>
         <v>420000</v>
       </c>
-      <c r="J7" s="8" t="str">
-        <f>VLOOKUP(J5, config!$B$4:$C$12,2,FALSE) &amp; " - Single"</f>
+      <c r="L7" s="8" t="str">
+        <f>VLOOKUP(L5, config!$B$4:$C$14,2,FALSE) &amp; " - Single"</f>
         <v>Carbon budget 420 Mt - Single</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E8" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>T-A*INT*</v>
+      </c>
+      <c r="F8" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>2018-2050</v>
+      </c>
+      <c r="J8" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -2236,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,39 +2303,40 @@
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="19.140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8"/>
-    <col min="5" max="5" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="5" width="9.140625" style="8"/>
+    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G4" s="8" t="str">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2290,25 +2347,31 @@
         <v>74</v>
       </c>
       <c r="E5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>72</v>
       </c>
@@ -2318,47 +2381,71 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B5, config!$B$4:$C$12,2,FALSE) &amp; "_Multi"</f>
+        <f>VLOOKUP(B5, config!$B$4:$C$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_CB-420Mt_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C5, config!$B$4:$C$12,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D5, config!$B$4:$C$12,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
-      <c r="E7" s="8" t="str">
-        <f>VLOOKUP(E5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="F7" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
         <v>2018-2050</v>
       </c>
-      <c r="F7" s="8" t="str">
-        <f>VLOOKUP(F5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="G7" s="8" t="str">
+        <f>VLOOKUP(G5, config!$B$4:$C$14,2,FALSE)</f>
         <v>NET</v>
       </c>
-      <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="H7" s="8" t="str">
+        <f>VLOOKUP(H5, config!$B$4:$C$14,2,FALSE)</f>
         <v>UP</v>
       </c>
-      <c r="H7" s="8">
-        <f>VLOOKUP(H5, config!$B$4:$C$12,2,FALSE)</f>
+      <c r="I7" s="8">
+        <f>VLOOKUP(I5, config!$B$4:$C$14,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="I7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$C$12,2,FALSE)*1000</f>
+      <c r="K7" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$C$14,2,FALSE)*1000</f>
         <v>420000</v>
       </c>
-      <c r="J7" s="8" t="str">
-        <f>VLOOKUP(J5, config!$B$4:$C$12,2,FALSE) &amp; " - Multi"</f>
+      <c r="L7" s="8" t="str">
+        <f>VLOOKUP(L5, config!$B$4:$C$14,2,FALSE) &amp; " - Multi"</f>
         <v>Carbon budget 420 Mt - Multi</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E8" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>T-A*INT*</v>
+      </c>
+      <c r="F8" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>2018-2050</v>
+      </c>
+      <c r="J8" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$C$14,2,FALSE)</f>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust the CB 420 Mt CO2 case
- exclude navigation
- apply 420 Mt CO2 CB to 2018-2050 and 0 thereafter
- exclude CO2 bound
- allow negative balance for PWRCO2N
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget_420Mt.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9CF55B-7986-4970-B0AE-A09CEF1D4C6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8ECF0F-456A-444F-A081-0FFA32D74483}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="config" sheetId="20" r:id="rId2"/>
     <sheet name="single" sheetId="21" r:id="rId3"/>
     <sheet name="multi" sheetId="22" r:id="rId4"/>
+    <sheet name="negative_CO2" sheetId="23" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -36,7 +37,7 @@
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>LimType</t>
   </si>
@@ -348,7 +349,28 @@
     <t>Pset_PN</t>
   </si>
   <si>
-    <t>T-A*INT*</t>
+    <t>T-A*INT*,T-NAV*</t>
+  </si>
+  <si>
+    <t>2051-2100</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>COM_BNDNET</t>
+  </si>
+  <si>
+    <t>PWRCO2N</t>
   </si>
 </sst>
 </file>
@@ -360,7 +382,7 @@
     <numFmt numFmtId="164" formatCode="???,???.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,8 +479,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +524,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,7 +674,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -655,6 +696,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="5x indented GHG Textfiels" xfId="3" xr:uid="{5F614CE9-C529-4323-B893-6D57470EC2CB}"/>
@@ -1091,7 +1136,7 @@
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,15 +1902,16 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="9.140625" style="8"/>
+    <col min="3" max="3" width="30.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="9.140625" style="8"/>
     <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="8"/>
@@ -1934,10 +1980,13 @@
         <v>61</v>
       </c>
       <c r="C4" s="8" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN("",TRUE,"UC_CB-",C7,"Mt")</f>
-        <v>UC_CB-420Mt</v>
-      </c>
-      <c r="D4"/>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","CB",C7,"Mt",C6)</f>
+        <v>UC_CB_420_Mt_2018-2050</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","CB",D7,"Mt",D6)</f>
+        <v>UC_CB_0_Mt_2051-2100</v>
+      </c>
       <c r="E4"/>
       <c r="F4"/>
       <c r="G4"/>
@@ -1958,10 +2007,13 @@
         <v>69</v>
       </c>
       <c r="C5" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Carbon budget",C7,"Mt")</f>
-        <v>Carbon budget 420 Mt</v>
-      </c>
-      <c r="D5"/>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Carbon budget",C7,"Mt",C6)</f>
+        <v>Carbon budget 420 Mt 2018-2050</v>
+      </c>
+      <c r="D5" s="8" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Carbon budget",D7,"Mt",D6)</f>
+        <v>Carbon budget 0 Mt 2051-2100</v>
+      </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>
@@ -1983,6 +2035,9 @@
       <c r="C6" s="8" t="s">
         <v>68</v>
       </c>
+      <c r="D6" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -1991,6 +2046,9 @@
       <c r="C7" s="8">
         <v>420</v>
       </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
@@ -1999,6 +2057,9 @@
       <c r="C8" s="8" t="s">
         <v>84</v>
       </c>
+      <c r="D8" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -2007,6 +2068,9 @@
       <c r="C9" s="8" t="s">
         <v>81</v>
       </c>
+      <c r="D9" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
@@ -2015,6 +2079,9 @@
       <c r="C10" s="8" t="s">
         <v>80</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
@@ -2023,6 +2090,9 @@
       <c r="C11" s="8" t="s">
         <v>79</v>
       </c>
+      <c r="D11" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
@@ -2031,12 +2101,18 @@
       <c r="C12" s="8" t="s">
         <v>71</v>
       </c>
+      <c r="D12" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C13" s="8">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="8">
         <v>-1</v>
       </c>
     </row>
@@ -2048,7 +2124,9 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
@@ -2128,18 +2206,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="8"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="8"/>
@@ -2226,61 +2305,121 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B5, config!$B$4:$C$14,2,FALSE) &amp; "_Single"</f>
-        <v>UC_CB-420Mt_Single</v>
+        <f>VLOOKUP($B$5, config!$B$4:$D$14,2,FALSE) &amp; "_Single"</f>
+        <v>UC_CB_420_Mt_2018-2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>2018-2050</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>NET</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f>VLOOKUP(H5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>UP</v>
       </c>
       <c r="I7" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$C$14,2,FALSE)*1000</f>
+        <f>VLOOKUP("Value", config!$B$4:$D$14,2,FALSE)*1000</f>
         <v>420000</v>
       </c>
       <c r="L7" s="8" t="str">
-        <f>VLOOKUP(L5, config!$B$4:$C$14,2,FALSE) &amp; " - Single"</f>
-        <v>Carbon budget 420 Mt - Single</v>
+        <f>VLOOKUP($L$5, config!$B$4:$D$14,2,FALSE) &amp; " - Single"</f>
+        <v>Carbon budget 420 Mt 2018-2050 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>T-A*INT*</v>
+        <f>VLOOKUP(E$5, config!$B$4:$D$14,2,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>2018-2050</v>
       </c>
       <c r="J8" s="8">
-        <f>VLOOKUP(J$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(J$5, config!$B$4:$D$14,2,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="str">
+        <f>VLOOKUP($B$5, config!$B$4:$D$14,3,FALSE) &amp; "_Single"</f>
+        <v>UC_CB_0_Mt_2051-2100_Single</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>2051-2100</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>NET</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f>VLOOKUP(H$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="I9" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$D$14,3,FALSE)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f>VLOOKUP($L$5, config!$B$4:$D$14,3,FALSE) &amp; " - Single"</f>
+        <v>Carbon budget 0 Mt 2051-2100 - Single</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>2051-2100</v>
+      </c>
+      <c r="J10" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$D$14,3,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
@@ -2292,25 +2431,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="19.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="8"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="8"/>
     <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
@@ -2390,61 +2530,121 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B5, config!$B$4:$C$14,2,FALSE) &amp; "_Multi"</f>
-        <v>UC_CB-420Mt_Multi</v>
+        <f>VLOOKUP(B$5, config!$B$4:$D$14,2,FALSE) &amp; "_Multi"</f>
+        <v>UC_CB_420_Mt_2018-2050_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>2018-2050</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>NET</v>
       </c>
       <c r="H7" s="8" t="str">
-        <f>VLOOKUP(H5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>UP</v>
       </c>
       <c r="I7" s="8">
-        <f>VLOOKUP(I5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="K7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$C$14,2,FALSE)*1000</f>
+        <f>VLOOKUP("Value", config!$B$4:$D$14,2,FALSE)*1000</f>
         <v>420000</v>
       </c>
       <c r="L7" s="8" t="str">
-        <f>VLOOKUP(L5, config!$B$4:$C$14,2,FALSE) &amp; " - Multi"</f>
-        <v>Carbon budget 420 Mt - Multi</v>
+        <f>VLOOKUP(L$5, config!$B$4:$D$14,2,FALSE) &amp; " - Multi"</f>
+        <v>Carbon budget 420 Mt 2018-2050 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$C$14,2,FALSE)</f>
-        <v>T-A*INT*</v>
+        <f>VLOOKUP(E$5, config!$B$4:$D$14,2,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8" t="str">
-        <f>VLOOKUP(F$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,2,FALSE)</f>
         <v>2018-2050</v>
       </c>
       <c r="J8" s="8">
-        <f>VLOOKUP(J$5, config!$B$4:$C$14,2,FALSE)</f>
+        <f>VLOOKUP(J$5, config!$B$4:$D$14,2,FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="str">
+        <f>VLOOKUP(B$5, config!$B$4:$D$14,3,FALSE) &amp; "_Multi"</f>
+        <v>UC_CB_0_Mt_2051-2100_Multi</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D9" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>2051-2100</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f>VLOOKUP(G$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>NET</v>
+      </c>
+      <c r="H9" s="8" t="str">
+        <f>VLOOKUP(H$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="I9" s="8">
+        <f>VLOOKUP(I$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="K9" s="8">
+        <f>VLOOKUP("Value", config!$B$4:$D$14,3,FALSE)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="8" t="str">
+        <f>VLOOKUP(L$5, config!$B$4:$D$14,3,FALSE) &amp; " - Multi"</f>
+        <v>Carbon budget 0 Mt 2051-2100 - Multi</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="str">
+        <f>VLOOKUP(C$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f>VLOOKUP(D$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f>VLOOKUP(E$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f>VLOOKUP(F$5, config!$B$4:$D$14,3,FALSE)</f>
+        <v>2051-2100</v>
+      </c>
+      <c r="J10" s="8">
+        <f>VLOOKUP(J$5, config!$B$4:$D$14,3,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
@@ -2452,4 +2652,83 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2314F01-B0DB-448B-9217-DEB90E2D1CCA}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="18" t="str">
+        <f>Regions!C3</f>
+        <v>IE</v>
+      </c>
+      <c r="H3" s="18" t="str">
+        <f>Regions!D3</f>
+        <v>National</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="19">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="19">
+        <f>G4</f>
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>